<commit_message>
Add whole blood, analyte, h&e manifest
</commit_message>
<xml_diff>
--- a/template_examples/pbmc.xlsx
+++ b/template_examples/pbmc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priti/Documents/GIT/schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF09735-C780-144A-B886-B92BC5D4E56E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1DF5C2-B9A2-9D42-8AC1-B141904FD611}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -803,9 +803,6 @@
     <t>EDTA Tube</t>
   </si>
   <si>
-    <t>ml</t>
-  </si>
-  <si>
     <t>FFPE block #52</t>
   </si>
   <si>
@@ -837,6 +834,9 @@
   </si>
   <si>
     <t>Green-top Tube - Plasma (Olink)</t>
+  </si>
+  <si>
+    <t>mL</t>
   </si>
 </sst>
 </file>
@@ -1292,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1488,7 +1488,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2159,16 +2159,16 @@
         <v>100</v>
       </c>
       <c r="S23" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="T23">
         <v>10</v>
       </c>
       <c r="U23" t="s">
+        <v>62</v>
+      </c>
+      <c r="V23" t="s">
         <v>63</v>
-      </c>
-      <c r="V23" t="s">
-        <v>64</v>
       </c>
       <c r="W23">
         <v>123</v>
@@ -2180,13 +2180,13 @@
         <v>100</v>
       </c>
       <c r="Z23" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA23" t="s">
         <v>65</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="AB23" t="s">
         <v>66</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
@@ -2245,16 +2245,16 @@
         <v>100</v>
       </c>
       <c r="S24" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="T24">
         <v>10</v>
       </c>
       <c r="U24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="W24">
         <v>123</v>
@@ -2266,13 +2266,13 @@
         <v>100</v>
       </c>
       <c r="Z24" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA24" t="s">
         <v>65</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AB24" t="s">
         <v>66</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
@@ -2331,16 +2331,16 @@
         <v>100</v>
       </c>
       <c r="S25" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="T25">
         <v>10</v>
       </c>
       <c r="U25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="W25">
         <v>123</v>
@@ -2352,13 +2352,13 @@
         <v>100</v>
       </c>
       <c r="Z25" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA25" t="s">
         <v>65</v>
       </c>
-      <c r="AA25" t="s">
+      <c r="AB25" t="s">
         <v>66</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
@@ -2417,16 +2417,16 @@
         <v>100</v>
       </c>
       <c r="S26" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="T26">
         <v>10</v>
       </c>
       <c r="U26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W26">
         <v>123</v>
@@ -2438,13 +2438,13 @@
         <v>100</v>
       </c>
       <c r="Z26" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA26" t="s">
         <v>65</v>
       </c>
-      <c r="AA26" t="s">
+      <c r="AB26" t="s">
         <v>66</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
@@ -2503,16 +2503,16 @@
         <v>100</v>
       </c>
       <c r="S27" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="T27">
         <v>10</v>
       </c>
       <c r="U27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W27">
         <v>123</v>
@@ -2524,13 +2524,13 @@
         <v>100</v>
       </c>
       <c r="Z27" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA27" t="s">
         <v>65</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AB27" t="s">
         <v>66</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
@@ -2589,16 +2589,16 @@
         <v>100</v>
       </c>
       <c r="S28" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="T28">
         <v>10</v>
       </c>
       <c r="U28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W28">
         <v>123</v>
@@ -2610,13 +2610,13 @@
         <v>100</v>
       </c>
       <c r="Z28" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA28" t="s">
         <v>65</v>
       </c>
-      <c r="AA28" t="s">
+      <c r="AB28" t="s">
         <v>66</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">

</xml_diff>